<commit_message>
split out excel writer
</commit_message>
<xml_diff>
--- a/src/template/Book1.xlsx
+++ b/src/template/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hiepnh\spring\ExcelIOApachePOI\src\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EF507A-2680-4CBC-8AB5-E40654372811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E8E904-9C86-47F4-9633-E053F7B29513}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12915" activeTab="1" xr2:uid="{F100997F-85DD-4643-859A-C29C337BBCC8}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>